<commit_message>
refactoring, financial modeling ch2
refactoring, financial modeling ch2
</commit_message>
<xml_diff>
--- a/Quantitative Trading/demo_sheet.xlsx
+++ b/Quantitative Trading/demo_sheet.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="2">
   <si>
     <t>a</t>
   </si>
@@ -80,13 +80,37 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="62">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="4"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="5"/>
+    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1">
       <alignment wrapText="true"/>
     </xf>
@@ -252,34 +276,34 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="55" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="48" t="n">
+      <c r="A2" s="56" t="n">
         <v>1.0</v>
       </c>
-      <c r="B2" s="51" t="n">
+      <c r="B2" s="59" t="n">
         <v>4.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="49" t="n">
+      <c r="A3" s="57" t="n">
         <v>2.0</v>
       </c>
-      <c r="B3" s="52" t="n">
+      <c r="B3" s="60" t="n">
         <v>5.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="50" t="n">
+      <c r="A4" s="58" t="n">
         <v>3.0</v>
       </c>
-      <c r="B4" s="53" t="n">
+      <c r="B4" s="61" t="n">
         <v>6.0</v>
       </c>
     </row>

</xml_diff>